<commit_message>
got new lat scale rich for model results
</commit_message>
<xml_diff>
--- a/output/plots/table1.xlsx
+++ b/output/plots/table1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Fixed Effects</t>
   </si>
@@ -50,16 +50,7 @@
     <t>t value</t>
   </si>
   <si>
-    <t>Residuals</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t>Max</t>
+    <t>P value</t>
   </si>
 </sst>
 </file>
@@ -121,17 +112,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -146,6 +131,24 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,22 +430,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D8"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4"/>
+    <col min="1" max="1" width="40.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -454,92 +458,76 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>1.089</v>
-      </c>
-      <c r="C2" s="2">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>19.29</v>
+      <c r="B2" s="9">
+        <v>0.90759000000000001</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.184859</v>
+      </c>
+      <c r="D2" s="9">
+        <v>18.5</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2.5399999999999998E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>-0.22900000000000001</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-72.180000000000007</v>
+      <c r="B3" s="9">
+        <v>-0.20222899999999999</v>
+      </c>
+      <c r="C3" s="9">
+        <v>7.5398999999999994E-2</v>
+      </c>
+      <c r="D3" s="9">
+        <v>-36.4</v>
+      </c>
+      <c r="E3" s="10">
+        <v>7.7299999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>9.7000000000000003E-3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4.93</v>
+      <c r="B4" s="9">
+        <v>1.7028999999999999E-2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3.9045000000000003E-2</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3.74</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.66303999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>-3.3E-3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D5" s="2">
-        <v>-3.28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3">
-        <v>-5.73</v>
-      </c>
-      <c r="C8" s="3">
-        <v>-6.0000000000000001E-3</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4.4400000000000004</v>
+      <c r="B5" s="8">
+        <v>6.2820000000000003E-3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.7479999999999999E-2</v>
+      </c>
+      <c r="D5" s="12">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.71955999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>